<commit_message>
mappa aggiornata con nuovi concetti
</commit_message>
<xml_diff>
--- a/resources/conf/globalSettings - Test.xlsx
+++ b/resources/conf/globalSettings - Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariolepore/PycharmProjects/bio_ml_project/resources/conf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2591172-82F1-8548-AF42-EB20D474CB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9640670E-14DC-DB4C-B5D4-F1D7565F80E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="21800" windowHeight="12980" xr2:uid="{28E020B9-CBE0-D144-B12F-12C146EF3C67}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,13 +443,13 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="C3">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D3">
-        <v>55</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>